<commit_message>
adding turf data to upside for the regressions
</commit_message>
<xml_diff>
--- a/data/DiscoverTURFs_simple.xlsx
+++ b/data/DiscoverTURFs_simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="14960" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="1620" yWindow="100" windowWidth="14960" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="162">
   <si>
     <t>Panulirus argus</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>Sarpa salpa</t>
+  </si>
+  <si>
+    <t>CatchShare</t>
   </si>
 </sst>
 </file>
@@ -922,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -934,7 +937,7 @@
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -944,8 +947,11 @@
       <c r="C1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -955,8 +961,11 @@
       <c r="C2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -966,8 +975,11 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -977,8 +989,11 @@
       <c r="C4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -988,8 +1003,11 @@
       <c r="C5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -999,8 +1017,11 @@
       <c r="C6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1010,8 +1031,11 @@
       <c r="C7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1021,8 +1045,11 @@
       <c r="C8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1032,8 +1059,11 @@
       <c r="C9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1043,8 +1073,11 @@
       <c r="C10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1054,8 +1087,11 @@
       <c r="C11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1065,8 +1101,11 @@
       <c r="C12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1076,8 +1115,11 @@
       <c r="C13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1087,8 +1129,11 @@
       <c r="C14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1098,8 +1143,11 @@
       <c r="C15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -1109,8 +1157,11 @@
       <c r="C16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1120,8 +1171,11 @@
       <c r="C17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1131,8 +1185,11 @@
       <c r="C18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1142,8 +1199,11 @@
       <c r="C19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1153,8 +1213,11 @@
       <c r="C20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1164,8 +1227,11 @@
       <c r="C21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1175,8 +1241,11 @@
       <c r="C22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1186,8 +1255,11 @@
       <c r="C23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1197,8 +1269,11 @@
       <c r="C24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1208,8 +1283,11 @@
       <c r="C25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1219,8 +1297,11 @@
       <c r="C26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1230,8 +1311,11 @@
       <c r="C27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -1241,8 +1325,11 @@
       <c r="C28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1252,8 +1339,11 @@
       <c r="C29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -1263,8 +1353,11 @@
       <c r="C30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1274,8 +1367,11 @@
       <c r="C31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1285,8 +1381,11 @@
       <c r="C32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1296,8 +1395,11 @@
       <c r="C33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1307,8 +1409,11 @@
       <c r="C34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -1318,8 +1423,11 @@
       <c r="C35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -1329,8 +1437,11 @@
       <c r="C36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -1340,8 +1451,11 @@
       <c r="C37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -1351,8 +1465,11 @@
       <c r="C38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -1362,8 +1479,11 @@
       <c r="C39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>62</v>
       </c>
@@ -1373,8 +1493,11 @@
       <c r="C40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>62</v>
       </c>
@@ -1384,8 +1507,11 @@
       <c r="C41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -1395,8 +1521,11 @@
       <c r="C42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -1406,8 +1535,11 @@
       <c r="C43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -1417,8 +1549,11 @@
       <c r="C44" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -1428,8 +1563,11 @@
       <c r="C45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>62</v>
       </c>
@@ -1439,8 +1577,11 @@
       <c r="C46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -1450,8 +1591,11 @@
       <c r="C47" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -1461,8 +1605,11 @@
       <c r="C48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -1472,8 +1619,11 @@
       <c r="C49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -1483,8 +1633,11 @@
       <c r="C50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -1494,8 +1647,11 @@
       <c r="C51" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -1505,8 +1661,11 @@
       <c r="C52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -1516,8 +1675,11 @@
       <c r="C53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -1527,8 +1689,11 @@
       <c r="C54" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -1538,8 +1703,11 @@
       <c r="C55" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -1549,8 +1717,11 @@
       <c r="C56" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -1560,8 +1731,11 @@
       <c r="C57" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -1571,8 +1745,11 @@
       <c r="C58" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -1582,8 +1759,11 @@
       <c r="C59" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -1593,8 +1773,11 @@
       <c r="C60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -1604,8 +1787,11 @@
       <c r="C61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -1615,8 +1801,11 @@
       <c r="C62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -1626,8 +1815,11 @@
       <c r="C63" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -1637,8 +1829,11 @@
       <c r="C64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>91</v>
       </c>
@@ -1648,8 +1843,11 @@
       <c r="C65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>91</v>
       </c>
@@ -1659,8 +1857,11 @@
       <c r="C66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -1670,8 +1871,11 @@
       <c r="C67" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>91</v>
       </c>
@@ -1681,8 +1885,11 @@
       <c r="C68" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>91</v>
       </c>
@@ -1692,8 +1899,11 @@
       <c r="C69" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>91</v>
       </c>
@@ -1703,8 +1913,11 @@
       <c r="C70" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -1714,8 +1927,11 @@
       <c r="C71" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>91</v>
       </c>
@@ -1725,8 +1941,11 @@
       <c r="C72" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>91</v>
       </c>
@@ -1736,8 +1955,11 @@
       <c r="C73" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -1747,8 +1969,11 @@
       <c r="C74" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>96</v>
       </c>
@@ -1758,8 +1983,11 @@
       <c r="C75" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -1769,8 +1997,11 @@
       <c r="C76" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>96</v>
       </c>
@@ -1780,8 +2011,11 @@
       <c r="C77" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -1791,8 +2025,11 @@
       <c r="C78" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -1802,8 +2039,11 @@
       <c r="C79" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>96</v>
       </c>
@@ -1813,8 +2053,11 @@
       <c r="C80" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>109</v>
       </c>
@@ -1824,8 +2067,11 @@
       <c r="C81" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>109</v>
       </c>
@@ -1835,8 +2081,11 @@
       <c r="C82" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>109</v>
       </c>
@@ -1846,8 +2095,11 @@
       <c r="C83" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>109</v>
       </c>
@@ -1857,8 +2109,11 @@
       <c r="C84" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -1868,8 +2123,11 @@
       <c r="C85" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>109</v>
       </c>
@@ -1879,8 +2137,11 @@
       <c r="C86" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>109</v>
       </c>
@@ -1890,8 +2151,11 @@
       <c r="C87" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
+      <c r="D87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>109</v>
       </c>
@@ -1901,8 +2165,11 @@
       <c r="C88" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>109</v>
       </c>
@@ -1912,8 +2179,11 @@
       <c r="C89" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>110</v>
       </c>
@@ -1923,8 +2193,11 @@
       <c r="C90" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
+      <c r="D90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>112</v>
       </c>
@@ -1934,8 +2207,11 @@
       <c r="C91" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
+      <c r="D91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>113</v>
       </c>
@@ -1945,8 +2221,11 @@
       <c r="C92" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>121</v>
       </c>
@@ -1956,8 +2235,11 @@
       <c r="C93" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>121</v>
       </c>
@@ -1967,8 +2249,11 @@
       <c r="C94" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="D94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>121</v>
       </c>
@@ -1978,8 +2263,11 @@
       <c r="C95" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>121</v>
       </c>
@@ -1989,8 +2277,11 @@
       <c r="C96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:3">
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>121</v>
       </c>
@@ -2000,8 +2291,11 @@
       <c r="C97" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:3">
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>121</v>
       </c>
@@ -2011,8 +2305,11 @@
       <c r="C98" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>121</v>
       </c>
@@ -2022,8 +2319,11 @@
       <c r="C99" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:3">
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>122</v>
       </c>
@@ -2033,8 +2333,11 @@
       <c r="C100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>123</v>
       </c>
@@ -2044,8 +2347,11 @@
       <c r="C101" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>130</v>
       </c>
@@ -2055,8 +2361,11 @@
       <c r="C102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:3">
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>130</v>
       </c>
@@ -2066,8 +2375,11 @@
       <c r="C103" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>130</v>
       </c>
@@ -2077,8 +2389,11 @@
       <c r="C104" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:3">
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>130</v>
       </c>
@@ -2088,8 +2403,11 @@
       <c r="C105" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="D105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>130</v>
       </c>
@@ -2099,8 +2417,11 @@
       <c r="C106" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>130</v>
       </c>
@@ -2110,8 +2431,11 @@
       <c r="C107" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>131</v>
       </c>
@@ -2121,8 +2445,11 @@
       <c r="C108" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:3">
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>132</v>
       </c>
@@ -2132,8 +2459,11 @@
       <c r="C109" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:3">
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>133</v>
       </c>
@@ -2143,8 +2473,11 @@
       <c r="C110" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:3">
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>158</v>
       </c>
@@ -2154,8 +2487,11 @@
       <c r="C111" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:3">
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>158</v>
       </c>
@@ -2165,8 +2501,11 @@
       <c r="C112" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>158</v>
       </c>
@@ -2176,8 +2515,11 @@
       <c r="C113" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>158</v>
       </c>
@@ -2187,8 +2529,11 @@
       <c r="C114" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>158</v>
       </c>
@@ -2198,8 +2543,11 @@
       <c r="C115" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>158</v>
       </c>
@@ -2209,8 +2557,11 @@
       <c r="C116" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:3">
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>158</v>
       </c>
@@ -2220,8 +2571,11 @@
       <c r="C117" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:3">
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>158</v>
       </c>
@@ -2231,8 +2585,11 @@
       <c r="C118" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>158</v>
       </c>
@@ -2242,8 +2599,11 @@
       <c r="C119" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:3">
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>158</v>
       </c>
@@ -2253,8 +2613,11 @@
       <c r="C120" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>158</v>
       </c>
@@ -2264,8 +2627,11 @@
       <c r="C121" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>136</v>
       </c>
@@ -2275,8 +2641,11 @@
       <c r="C122" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>136</v>
       </c>
@@ -2286,8 +2655,11 @@
       <c r="C123" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>136</v>
       </c>
@@ -2297,8 +2669,11 @@
       <c r="C124" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>136</v>
       </c>
@@ -2308,8 +2683,11 @@
       <c r="C125" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:3">
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>136</v>
       </c>
@@ -2319,8 +2697,11 @@
       <c r="C126" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
+      <c r="D126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>149</v>
       </c>
@@ -2330,8 +2711,11 @@
       <c r="C127" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:3">
+      <c r="D127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>149</v>
       </c>
@@ -2341,8 +2725,11 @@
       <c r="C128" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>149</v>
       </c>
@@ -2352,8 +2739,11 @@
       <c r="C129" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>149</v>
       </c>
@@ -2363,8 +2753,11 @@
       <c r="C130" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="D130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>149</v>
       </c>
@@ -2374,8 +2767,11 @@
       <c r="C131" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="D131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>149</v>
       </c>
@@ -2385,8 +2781,11 @@
       <c r="C132" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="D132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>149</v>
       </c>
@@ -2396,8 +2795,11 @@
       <c r="C133" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="D133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -2407,8 +2809,11 @@
       <c r="C134" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="D134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>88</v>
       </c>
@@ -2418,8 +2823,11 @@
       <c r="C135" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="D135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>88</v>
       </c>
@@ -2429,8 +2837,11 @@
       <c r="C136" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="D136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>88</v>
       </c>
@@ -2440,8 +2851,11 @@
       <c r="C137" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="D137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>88</v>
       </c>
@@ -2451,8 +2865,11 @@
       <c r="C138" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="D138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>88</v>
       </c>
@@ -2462,8 +2879,11 @@
       <c r="C139" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="D139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>88</v>
       </c>
@@ -2473,8 +2893,11 @@
       <c r="C140" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>88</v>
       </c>
@@ -2484,8 +2907,11 @@
       <c r="C141" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>88</v>
       </c>
@@ -2495,8 +2921,11 @@
       <c r="C142" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>88</v>
       </c>
@@ -2506,8 +2935,11 @@
       <c r="C143" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="D143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>88</v>
       </c>
@@ -2517,8 +2949,11 @@
       <c r="C144" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="D144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>88</v>
       </c>
@@ -2526,6 +2961,9 @@
         <v>22</v>
       </c>
       <c r="C145" t="b">
+        <v>1</v>
+      </c>
+      <c r="D145">
         <v>1</v>
       </c>
     </row>

</xml_diff>